<commit_message>
update after conceptual meeting
</commit_message>
<xml_diff>
--- a/data/excel/resourceType.xlsx
+++ b/data/excel/resourceType.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\moon.ntkcz.cz\petka\NUŠL\SW\INVENIO 3\taxonomie\současné_hotové\NR_docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cernohlp\Documents\GitHub\nr-taxonomies\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,42 +23,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Petra Černohlávková</author>
-  </authors>
-  <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t>Petra Černohlávková:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t xml:space="preserve">
-v případě dvou taxonomií, potřebují o sobě vědět? Mapování stejných kategorií kvůli lepší práci s related item?</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="173">
   <si>
@@ -152,9 +116,6 @@
     <t>trade-literature</t>
   </si>
   <si>
-    <t>theses-(etds)</t>
-  </si>
-  <si>
     <t>methodologies-and-procedures</t>
   </si>
   <si>
@@ -434,33 +395,6 @@
     <t>review</t>
   </si>
   <si>
-    <t>conference-paper</t>
-  </si>
-  <si>
-    <t>conference-proceeding</t>
-  </si>
-  <si>
-    <t>conference-programme</t>
-  </si>
-  <si>
-    <t>conference-poster</t>
-  </si>
-  <si>
-    <t>bachelor-thesis</t>
-  </si>
-  <si>
-    <t>master-thesis</t>
-  </si>
-  <si>
-    <t>rigorous-thesis</t>
-  </si>
-  <si>
-    <t>doctoral-thesis</t>
-  </si>
-  <si>
-    <t>post-doctoral-thesis</t>
-  </si>
-  <si>
     <t>certified-methodology</t>
   </si>
   <si>
@@ -473,24 +407,6 @@
     <t>treatment-procedure</t>
   </si>
   <si>
-    <t>annual-report</t>
-  </si>
-  <si>
-    <t>research-report</t>
-  </si>
-  <si>
-    <t>project-report</t>
-  </si>
-  <si>
-    <t>conservation-report</t>
-  </si>
-  <si>
-    <t>field-report</t>
-  </si>
-  <si>
-    <t>business-trip-report</t>
-  </si>
-  <si>
     <t>press-release</t>
   </si>
   <si>
@@ -500,9 +416,6 @@
     <t>educational-material</t>
   </si>
   <si>
-    <t>statistical-or-status-report</t>
-  </si>
-  <si>
     <t>exhibition-catalogue-or-guide</t>
   </si>
   <si>
@@ -579,13 +492,64 @@
   </si>
   <si>
     <t>nonpreferredLabels_en_0</t>
+  </si>
+  <si>
+    <t>paper</t>
+  </si>
+  <si>
+    <t>proceeding</t>
+  </si>
+  <si>
+    <t>programme</t>
+  </si>
+  <si>
+    <t>poster</t>
+  </si>
+  <si>
+    <t>theses</t>
+  </si>
+  <si>
+    <t>bachelor</t>
+  </si>
+  <si>
+    <t>master</t>
+  </si>
+  <si>
+    <t>rigorous</t>
+  </si>
+  <si>
+    <t>doctoral</t>
+  </si>
+  <si>
+    <t>post-doctoral</t>
+  </si>
+  <si>
+    <t>annual</t>
+  </si>
+  <si>
+    <t>research</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>statistical-or-status</t>
+  </si>
+  <si>
+    <t>conservation</t>
+  </si>
+  <si>
+    <t>field</t>
+  </si>
+  <si>
+    <t>business-trip</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -628,21 +592,6 @@
       <charset val="238"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -650,18 +599,12 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -716,11 +659,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hypertextový odkaz" xfId="2" builtinId="8"/>
@@ -1002,12 +945,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H5" sqref="H5"/>
+      <selection pane="topRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1034,7 +977,7 @@
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="18" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
@@ -1069,19 +1012,19 @@
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -1089,25 +1032,25 @@
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -1115,25 +1058,25 @@
         <v>1</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E7" t="s">
         <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I7" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -1141,46 +1084,46 @@
         <v>1</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="J8" s="17"/>
+        <v>44</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="J8" s="16"/>
     </row>
     <row r="9" spans="1:10" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>1</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>160</v>
+        <v>138</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -1188,33 +1131,33 @@
         <v>1</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="I10" s="16" t="s">
         <v>63</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>1</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="6" t="s">
@@ -1229,22 +1172,22 @@
         <v>2</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>124</v>
+        <v>156</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="H12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I12" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -1252,22 +1195,22 @@
         <v>2</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="H13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I13" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -1275,22 +1218,22 @@
         <v>2</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>126</v>
+        <v>158</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="H14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -1298,33 +1241,33 @@
         <v>2</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>127</v>
+        <v>159</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="H15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>1</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>30</v>
+      <c r="B16" s="11" t="s">
+        <v>160</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>25</v>
@@ -1342,22 +1285,22 @@
         <v>2</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>128</v>
+        <v>161</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I17" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="J17" s="8"/>
     </row>
@@ -1366,22 +1309,22 @@
         <v>2</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>129</v>
+        <v>162</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I18" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="J18" s="8"/>
     </row>
@@ -1390,25 +1333,25 @@
         <v>2</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>130</v>
+        <v>163</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I19" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="J19" s="8"/>
     </row>
@@ -1417,25 +1360,25 @@
         <v>2</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>131</v>
+        <v>164</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I20" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="J20" s="8"/>
     </row>
@@ -1444,33 +1387,33 @@
         <v>2</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>132</v>
+        <v>165</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I21" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>1</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>31</v>
+      <c r="B22" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>20</v>
@@ -1484,22 +1427,22 @@
         <v>2</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I23" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -1507,22 +1450,22 @@
         <v>2</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I24" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -1530,25 +1473,25 @@
         <v>2</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="F25" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="G25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I25" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -1556,29 +1499,29 @@
         <v>2</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I26" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>1</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="6" t="s">
@@ -1593,22 +1536,22 @@
         <v>2</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="H28" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="I28" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -1616,22 +1559,22 @@
         <v>2</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I29" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -1639,22 +1582,22 @@
         <v>2</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="C30" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="H30" t="s">
+        <v>153</v>
+      </c>
+      <c r="I30" t="s">
         <v>148</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="H30" t="s">
-        <v>170</v>
-      </c>
-      <c r="I30" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -1662,25 +1605,25 @@
         <v>2</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="H31" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="I31" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1688,22 +1631,22 @@
         <v>2</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="H32" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="I32" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -1711,22 +1654,22 @@
         <v>2</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="H33" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="I33" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -1734,22 +1677,22 @@
         <v>2</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>142</v>
+        <v>172</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="H34" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="I34" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -1757,22 +1700,22 @@
         <v>2</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="H35" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="I35" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -1780,7 +1723,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>22</v>
@@ -1797,22 +1740,22 @@
         <v>29</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I37" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -1820,22 +1763,22 @@
         <v>2</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="G38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I38" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -1843,22 +1786,22 @@
         <v>2</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -1866,22 +1809,22 @@
         <v>2</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="C40" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="I40" s="17" t="s">
-        <v>160</v>
+        <v>55</v>
+      </c>
+      <c r="I40" s="16" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -1889,22 +1832,22 @@
         <v>2</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="I41" s="17" t="s">
-        <v>160</v>
+        <v>55</v>
+      </c>
+      <c r="I41" s="16" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1912,24 +1855,24 @@
         <v>2</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C42" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D42" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>60</v>
       </c>
       <c r="E42"/>
       <c r="F42"/>
       <c r="G42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H42" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="I42" s="17" t="s">
-        <v>60</v>
+        <v>55</v>
+      </c>
+      <c r="I42" s="16" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -1968,7 +1911,7 @@
       <c r="B48" s="11"/>
       <c r="C48" s="14"/>
       <c r="D48" s="14"/>
-      <c r="I48" s="18"/>
+      <c r="I48" s="17"/>
     </row>
     <row r="49" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
@@ -2026,6 +1969,5 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId19"/>
-  <legacyDrawing r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>